<commit_message>
reading files with python
</commit_message>
<xml_diff>
--- a/spreadsheet_code/pyxl.xlsx
+++ b/spreadsheet_code/pyxl.xlsx
@@ -1,73 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cecd304\me\documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366DEBFF-27C1-457D-AF44-9DF2059781C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="8730" xr2:uid="{450EA59D-C06E-4DAE-A60D-00DC34DD4780}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19620" windowHeight="8730" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="LALALA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>apples</t>
-  </si>
-  <si>
-    <t>cherries</t>
-  </si>
-  <si>
-    <t>pears</t>
-  </si>
-  <si>
-    <t>oranges</t>
-  </si>
-  <si>
-    <t>bananas</t>
-  </si>
-  <si>
-    <t>strawberries</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -86,22 +48,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -401,142 +354,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A93D4B5-A222-4A62-8468-90A8EA57E281}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12.140625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="n">
         <v>43753</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>apples</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>43754</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>cherries</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>43755</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pears</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>43756</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>oranges</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>HELLO WORLD</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>43757</v>
       </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>apples</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>43758</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>bananas</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>43759</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>strawberries</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAFED1A-8506-4C22-8EFD-02C9690F1256}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1523AA-DE91-434E-84C9-AE1FCF82AAB2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>